<commit_message>
added fixed document and test case
</commit_message>
<xml_diff>
--- a/document/TestCase.xlsx
+++ b/document/TestCase.xlsx
@@ -867,12 +867,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -888,20 +888,22 @@
     </font>
     <font>
       <sz val="13"/>
-      <color theme="0"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="13"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -913,14 +915,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -942,11 +944,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -966,31 +968,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1006,16 +993,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1033,16 +1013,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1057,13 +1045,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1075,49 +1069,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1135,7 +1111,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1147,25 +1189,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1183,61 +1207,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1262,21 +1250,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1320,11 +1293,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1346,15 +1343,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1366,15 +1354,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1387,37 +1375,37 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1426,92 +1414,92 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1526,47 +1514,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1898,8 +1859,8 @@
   <sheetPr/>
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -1919,1346 +1880,1346 @@
       <c r="B1" s="7">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" ht="94" customHeight="1" spans="1:8">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="7">
         <f t="shared" ref="B2:B7" si="0">IF(C2&lt;&gt;"",B1+1,"")</f>
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" ht="84" spans="1:8">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11">
+      <c r="A3" s="8"/>
+      <c r="B3" s="7">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" ht="150" customHeight="1" spans="1:8">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11">
+      <c r="A4" s="8"/>
+      <c r="B4" s="7">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" ht="150" customHeight="1" spans="1:8">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11">
+      <c r="A5" s="8"/>
+      <c r="B5" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" ht="150" customHeight="1" spans="1:8">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11">
+      <c r="A6" s="8"/>
+      <c r="B6" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" ht="150" customHeight="1" spans="1:8">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11">
+      <c r="A7" s="8"/>
+      <c r="B7" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" ht="150" customHeight="1" spans="1:8">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11">
+      <c r="A8" s="8"/>
+      <c r="B8" s="7">
         <f t="shared" ref="B8:B10" si="1">IF(C8&lt;&gt;"",B6+1,"")</f>
         <v>6</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="150" customHeight="1" spans="1:8">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11">
+      <c r="A9" s="8"/>
+      <c r="B9" s="7">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" ht="150" customHeight="1" spans="1:8">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11">
+      <c r="A10" s="8"/>
+      <c r="B10" s="7">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="150" customHeight="1" spans="1:8">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11">
+      <c r="A11" s="8"/>
+      <c r="B11" s="7">
         <f t="shared" ref="B11:B14" si="2">IF(C11&lt;&gt;"",B10+1,"")</f>
         <v>8</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" ht="150" customHeight="1" spans="1:8">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11">
+      <c r="A12" s="8"/>
+      <c r="B12" s="7">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" ht="150" customHeight="1" spans="1:8">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11">
+      <c r="A13" s="8"/>
+      <c r="B13" s="7">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" ht="150" customHeight="1" spans="1:8">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11">
+      <c r="A14" s="8"/>
+      <c r="B14" s="7">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" ht="150" customHeight="1" spans="1:8">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11">
+      <c r="A15" s="8"/>
+      <c r="B15" s="7">
         <f t="shared" ref="B15:B17" si="3">IF(C15&lt;&gt;"",B13+1,"")</f>
         <v>11</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" ht="150" customHeight="1" spans="1:8">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11">
+      <c r="A16" s="8"/>
+      <c r="B16" s="7">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" ht="150" customHeight="1" spans="1:8">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11">
+      <c r="A17" s="8"/>
+      <c r="B17" s="7">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="1" ht="100.8" spans="1:8">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="11" t="e">
+      <c r="B18" s="7" t="e">
         <f>IF(C18&lt;&gt;"",#REF!+1,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="H18" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="1" ht="117.6" spans="1:8">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11" t="e">
+      <c r="A19" s="8"/>
+      <c r="B19" s="7" t="e">
         <f>IF(C19&lt;&gt;"",B18+1,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="84" spans="1:8">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11" t="e">
+      <c r="A20" s="8"/>
+      <c r="B20" s="7" t="e">
         <f>IF(C20&lt;&gt;"",B19+1,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" ht="84" spans="1:8">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11" t="e">
+      <c r="A21" s="8"/>
+      <c r="B21" s="7" t="e">
         <f>IF(C21&lt;&gt;"",B20+1,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" s="2" customFormat="1" ht="50.4" spans="1:8">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11" t="e">
+      <c r="A22" s="8"/>
+      <c r="B22" s="7" t="e">
         <f>IF(C22&lt;&gt;"",B21+1,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H22" s="13" t="s">
+      <c r="H22" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" s="2" customFormat="1" ht="67.2" spans="1:8">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12" t="s">
+      <c r="A23" s="8"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="H23" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" s="2" customFormat="1" ht="67.2" spans="1:8">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11" t="e">
+      <c r="A24" s="8"/>
+      <c r="B24" s="7" t="e">
         <f>IF(C24&lt;&gt;"",B22+1,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="G24" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" s="2" customFormat="1" ht="67.2" spans="1:8">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11" t="e">
+      <c r="A25" s="8"/>
+      <c r="B25" s="7" t="e">
         <f>IF(C25&lt;&gt;"",B24+1,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H25" s="13" t="s">
+      <c r="H25" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" s="2" customFormat="1" ht="33.6" spans="1:8">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11" t="e">
+      <c r="A26" s="8"/>
+      <c r="B26" s="7" t="e">
         <f>IF(C26&lt;&gt;"",B25+1,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="G26" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H26" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" s="2" customFormat="1" ht="67.2" spans="1:8">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="12" t="s">
+      <c r="A27" s="8"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" s="2" customFormat="1" ht="84" spans="1:8">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B28" s="11" t="e">
+      <c r="B28" s="7" t="e">
         <f>IF(C28&lt;&gt;"",B26+1,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="29" s="2" customFormat="1" ht="117.6" spans="1:8">
-      <c r="A29" s="10"/>
-      <c r="B29" s="11" t="e">
+      <c r="A29" s="8"/>
+      <c r="B29" s="7" t="e">
         <f>IF(C29&lt;&gt;"",B28+1,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="30" s="2" customFormat="1" ht="134.4" spans="1:8">
-      <c r="A30" s="10"/>
-      <c r="B30" s="11" t="e">
+      <c r="A30" s="8"/>
+      <c r="B30" s="7" t="e">
         <f>IF(C30&lt;&gt;"",B29+1,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H30" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="31" s="2" customFormat="1" ht="134.4" spans="1:8">
-      <c r="A31" s="10"/>
-      <c r="B31" s="11" t="e">
+      <c r="A31" s="8"/>
+      <c r="B31" s="7" t="e">
         <f>IF(C31&lt;&gt;"",B30+1,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="H31" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="32" s="2" customFormat="1" ht="100.8" spans="1:8">
-      <c r="A32" s="10"/>
-      <c r="B32" s="11" t="e">
+      <c r="A32" s="8"/>
+      <c r="B32" s="7" t="e">
         <f>IF(C32&lt;&gt;"",B31+1,"")</f>
         <v>#REF!</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="H32" s="13" t="s">
+      <c r="H32" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="33" s="2" customFormat="1" ht="201.6" spans="1:8">
-      <c r="A33" s="10"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="14" t="s">
+      <c r="A33" s="8"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="H33" s="13" t="s">
+      <c r="H33" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="34" s="2" customFormat="1" ht="134.4" spans="1:8">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="14" t="s">
+      <c r="A34" s="8"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="H34" s="13" t="s">
+      <c r="H34" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="35" s="2" customFormat="1" ht="151.2" spans="1:8">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17" t="s">
+      <c r="A35" s="8"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D35" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="E35" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F35" s="17" t="s">
+      <c r="F35" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="G35" s="17" t="s">
+      <c r="G35" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="H35" s="19" t="s">
+      <c r="H35" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="36" s="2" customFormat="1" ht="184.8" spans="1:8">
-      <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="17" t="s">
+      <c r="A36" s="8"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E36" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F36" s="17" t="s">
+      <c r="F36" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="G36" s="17" t="s">
+      <c r="G36" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="H36" s="19" t="s">
+      <c r="H36" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="37" s="2" customFormat="1" ht="151.2" spans="1:8">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="14" t="s">
+      <c r="A37" s="8"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F37" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="G37" s="14" t="s">
+      <c r="G37" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="H37" s="13" t="s">
+      <c r="H37" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="38" s="2" customFormat="1" ht="184.8" spans="1:8">
-      <c r="A38" s="10"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="14" t="s">
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="G38" s="17" t="s">
+      <c r="G38" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="H38" s="13" t="s">
+      <c r="H38" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="39" s="2" customFormat="1" ht="84" spans="1:8">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="14" t="s">
+      <c r="B39" s="7"/>
+      <c r="C39" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D39" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="G39" s="14" t="s">
+      <c r="G39" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="H39" s="13" t="s">
+      <c r="H39" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="40" s="2" customFormat="1" ht="84" spans="1:8">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="14" t="s">
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="G40" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H40" s="13" t="s">
+      <c r="H40" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="41" s="2" customFormat="1" ht="84" spans="1:8">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="14" t="s">
+      <c r="B41" s="7"/>
+      <c r="C41" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="F41" s="14" t="s">
+      <c r="F41" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="G41" s="14" t="s">
+      <c r="G41" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="H41" s="13" t="s">
+      <c r="H41" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="42" s="2" customFormat="1" ht="84" spans="1:8">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="14" t="s">
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="F42" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="H42" s="13" t="s">
+      <c r="H42" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="43" s="2" customFormat="1" ht="84" spans="1:8">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="14" t="s">
+      <c r="B43" s="7"/>
+      <c r="C43" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D43" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F43" s="14" t="s">
+      <c r="F43" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="G43" s="14" t="s">
+      <c r="G43" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="H43" s="13" t="s">
+      <c r="H43" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="44" s="2" customFormat="1" ht="84" spans="1:8">
-      <c r="A44" s="10"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="14" t="s">
+      <c r="A44" s="8"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="F44" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="G44" s="14" t="s">
+      <c r="G44" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="H44" s="13" t="s">
+      <c r="H44" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="45" s="2" customFormat="1" ht="100.8" spans="1:8">
-      <c r="A45" s="10"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="14" t="s">
+      <c r="A45" s="8"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="D45" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E45" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="F45" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="G45" s="14" t="s">
+      <c r="G45" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="H45" s="13" t="s">
+      <c r="H45" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="46" s="2" customFormat="1" ht="117.6" spans="1:8">
-      <c r="A46" s="10"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="14" t="s">
+      <c r="A46" s="8"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="D46" s="14" t="s">
+      <c r="D46" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F46" s="14" t="s">
+      <c r="F46" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="G46" s="14" t="s">
+      <c r="G46" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="H46" s="13" t="s">
+      <c r="H46" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="47" s="2" customFormat="1" ht="117.6" spans="1:8">
-      <c r="A47" s="10"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="14" t="s">
+      <c r="A47" s="8"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="D47" s="14" t="s">
+      <c r="D47" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E47" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="F47" s="14" t="s">
+      <c r="F47" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="G47" s="14" t="s">
+      <c r="G47" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="H47" s="13" t="s">
+      <c r="H47" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="48" s="2" customFormat="1" ht="151.2" spans="1:8">
-      <c r="A48" s="10"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="14" t="s">
+      <c r="A48" s="8"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="D48" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E48" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="F48" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="G48" s="14" t="s">
+      <c r="G48" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="H48" s="13" t="s">
+      <c r="H48" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="49" s="2" customFormat="1" ht="117.6" spans="1:8">
-      <c r="A49" s="10"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="14" t="s">
+      <c r="A49" s="8"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="D49" s="14" t="s">
+      <c r="D49" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="F49" s="14" t="s">
+      <c r="F49" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="G49" s="14" t="s">
+      <c r="G49" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="H49" s="13" t="s">
+      <c r="H49" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="50" s="2" customFormat="1" ht="134.4" spans="1:8">
-      <c r="A50" s="10"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="14" t="s">
+      <c r="A50" s="8"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="D50" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F50" s="14" t="s">
+      <c r="F50" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="G50" s="14" t="s">
+      <c r="G50" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="H50" s="13" t="s">
+      <c r="H50" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="51" s="2" customFormat="1" ht="100.8" spans="1:8">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="14" t="s">
+      <c r="B51" s="7"/>
+      <c r="C51" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="D51" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E51" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="F51" s="14" t="s">
+      <c r="F51" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="G51" s="14" t="s">
+      <c r="G51" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="H51" s="13" t="s">
+      <c r="H51" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="52" s="2" customFormat="1" ht="117.6" spans="1:8">
-      <c r="A52" s="10"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="14" t="s">
+      <c r="A52" s="8"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="F52" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="G52" s="14" t="s">
+      <c r="G52" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="H52" s="13" t="s">
+      <c r="H52" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="53" s="2" customFormat="1" ht="84" spans="1:8">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="14" t="s">
+      <c r="B53" s="7"/>
+      <c r="C53" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E53" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="F53" s="14" t="s">
+      <c r="F53" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="G53" s="14" t="s">
+      <c r="G53" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="H53" s="13" t="s">
+      <c r="H53" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="54" ht="134.4" spans="1:8">
-      <c r="A54" s="10"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="14" t="s">
+      <c r="A54" s="8"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E54" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="F54" s="14" t="s">
+      <c r="F54" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="G54" s="14" t="s">
+      <c r="G54" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="H54" s="13" t="s">
+      <c r="H54" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="55" ht="134.4" spans="1:8">
-      <c r="A55" s="10"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="14" t="s">
+      <c r="A55" s="8"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="E55" s="12" t="s">
+      <c r="E55" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="F55" s="14" t="s">
+      <c r="F55" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="G55" s="14" t="s">
+      <c r="G55" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="H55" s="13" t="s">
+      <c r="H55" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="56" ht="168" spans="1:8">
-      <c r="A56" s="10"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="14" t="s">
+      <c r="A56" s="8"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="D56" s="14" t="s">
+      <c r="D56" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="E56" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="F56" s="14" t="s">
+      <c r="F56" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="G56" s="14" t="s">
+      <c r="G56" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="H56" s="13" t="s">
+      <c r="H56" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="57" ht="16.8" spans="1:7">
       <c r="A57" s="2"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>